<commit_message>
update codebook based on experiences from praxisproject
</commit_message>
<xml_diff>
--- a/doc/codebook_compact.overview.file.xlsx
+++ b/doc/codebook_compact.overview.file.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projekte\Occupation Coding\occupationmeasurement-data-sharing\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9848B00F-B093-4751-9D2B-CA027AE4B2C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DEC7D87-E534-4DA3-8AFB-7CC52852D800}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{C7050F8A-CEB5-1D41-96C6-E33B10143149}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="468">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="474">
   <si>
     <t xml:space="preserve">Clarification </t>
   </si>
@@ -1030,9 +1030,6 @@
     <t>575 obs. Of 3 variables</t>
   </si>
   <si>
-    <t xml:space="preserve">Did interviewers (only those trained in conversational interviews could do so) toggle the detailled descriptions? </t>
-  </si>
-  <si>
     <t>2019-04-03 16:57:42</t>
   </si>
   <si>
@@ -1280,9 +1277,6 @@
   </si>
   <si>
     <t>After looking up the true code (kldb_auxco, isco_auxco), the professional coder could explain why her choice (kldb2010_kp, isco08_kp) deviates from the true code.</t>
-  </si>
-  <si>
-    <t>Columns Z to AL describe extensive reflections about the sources of error when the professional coder selects a KldB-/ISCO-code that is not the same as the one expected in AuxCO.</t>
   </si>
   <si>
     <t>ja</t>
@@ -1499,14 +1493,45 @@
   <si>
     <t xml:space="preserve">57 variables describe interviewer &amp; respondent behavior as they talk about two questions: 1. Welche berufliche Tätigkeit üben Sie derzeit hauptsächlich aus? 2. Welche der folgenden Beschreibungen trifft am ehesten für Ihren Beruf zu? This is not available for every interview, but only for a random(?) selection of 668 respondents who agreed to have their interview recorded and (I am not 100% sure about this:) were asked the question: Welche der folgenden Beschreibungen trifft am ehesten für Ihren Beruf zu?. </t>
   </si>
+  <si>
+    <t>Match</t>
+  </si>
+  <si>
+    <t>diese wird direkt in Excel berechnet: =(E1662=O1662)&amp;(G1662=Q1662) Dabei wird überprüft ob kldb_auxco == kldb2010_kp UND isco_auxco == isco08_kp. Wenn das Ergebnis TRUETRUE ist, stimmt der professionelle Kodierer mit den Codings aus der Auxco für die ISCO-Klassifikation und für die KldB-Klassifikation überein. Wenn das Ergebnis nicht TRUETRUE ist haben wir Abweichungen und haben dann versucht diese Fehlerquelle weiter zu verstehen.</t>
+  </si>
+  <si>
+    <t>Columns Z to AL describe extensive reflections about the sources of error when the professional coder selects a KldB-/ISCO-code that is not the same as the one expected in AuxCO. It is best to ignore these columns, because they are not useful for a statistical analysis.</t>
+  </si>
+  <si>
+    <t>kldb_beurteilung</t>
+  </si>
+  <si>
+    <t>isco_beurteilung</t>
+  </si>
+  <si>
+    <t>der professionelle Kodierer hat jeweils seine eigene Kodierung (z.B. kldb2010_kp) mit der AuxCo-Kodierung (z.b:  kldb_auxco) verglichen. Diese Spalten enthalten nun seine Beurteilung, welcher der beiden Codes zutreffender ist: 1 = Codierer findet seinen eigenen Code besser; 2 = Codierer findet beide Codes ähnlich gut; 3 = Codierer findet kldb_auxco-Code besser; NA=beide Codes sind identisch und es gibt nichts zu beurteilen.</t>
+  </si>
+  <si>
+    <t>like kldb_beurteilung, but for isco</t>
+  </si>
+  <si>
+    <t>Did interviewers (only those trained in conversational interviews could do so) toggle the detailled descriptions? That is, did they click on the text beneath an answer, such that detailed descriptions were opened?</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1606,17 +1631,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -1626,6 +1651,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1942,8 +1971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCCB7332-5145-44F1-AF2F-05E8E4AA4522}">
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5"/>
@@ -2123,13 +2152,13 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B23" t="s">
         <v>304</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E23" t="s">
         <v>305</v>
@@ -2137,19 +2166,19 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
+        <v>453</v>
+      </c>
+      <c r="B24" t="s">
+        <v>452</v>
+      </c>
+      <c r="C24" t="s">
+        <v>454</v>
+      </c>
+      <c r="D24" t="s">
         <v>455</v>
       </c>
-      <c r="B24" t="s">
-        <v>454</v>
-      </c>
-      <c r="C24" t="s">
+      <c r="E24" t="s">
         <v>456</v>
-      </c>
-      <c r="D24" t="s">
-        <v>457</v>
-      </c>
-      <c r="E24" t="s">
-        <v>458</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -2163,7 +2192,7 @@
         <v>302</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E25" t="s">
         <v>299</v>
@@ -2180,7 +2209,7 @@
         <v>306</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E26" t="s">
         <v>298</v>
@@ -2188,19 +2217,19 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
+        <v>363</v>
+      </c>
+      <c r="B28" t="s">
+        <v>451</v>
+      </c>
+      <c r="C28" t="s">
         <v>364</v>
       </c>
-      <c r="B28" t="s">
-        <v>453</v>
-      </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>365</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>366</v>
-      </c>
-      <c r="E28" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -2258,7 +2287,7 @@
         <v>5</v>
       </c>
       <c r="E34" t="s">
-        <v>324</v>
+        <v>473</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -2266,16 +2295,16 @@
         <v>320</v>
       </c>
       <c r="B35" t="s">
+        <v>331</v>
+      </c>
+      <c r="C35" t="s">
         <v>332</v>
-      </c>
-      <c r="C35" t="s">
-        <v>333</v>
       </c>
       <c r="D35" t="s">
         <v>5</v>
       </c>
       <c r="E35" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -2283,48 +2312,48 @@
         <v>320</v>
       </c>
       <c r="B36" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C36" t="s">
+        <v>336</v>
+      </c>
+      <c r="D36" t="s">
         <v>337</v>
       </c>
-      <c r="D36" t="s">
+      <c r="E36" t="s">
         <v>338</v>
-      </c>
-      <c r="E36" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="5" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="6" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" t="s">
+        <v>459</v>
+      </c>
+      <c r="B41" t="s">
+        <v>460</v>
+      </c>
+      <c r="C41" t="s">
         <v>461</v>
       </c>
-      <c r="B41" t="s">
-        <v>462</v>
-      </c>
-      <c r="C41" t="s">
-        <v>463</v>
-      </c>
       <c r="D41" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="E41" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="6" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
   </sheetData>
@@ -2836,7 +2865,7 @@
         <v>37</v>
       </c>
       <c r="C31" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="D31" t="s">
         <v>169</v>
@@ -2870,7 +2899,7 @@
         <v>38</v>
       </c>
       <c r="C33" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="D33" t="s">
         <v>177</v>
@@ -2887,7 +2916,7 @@
         <v>39</v>
       </c>
       <c r="C34" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="D34" t="s">
         <v>177</v>
@@ -3504,7 +3533,7 @@
     </row>
     <row r="87" spans="1:5">
       <c r="A87" s="5" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="88" spans="1:5">
@@ -3515,7 +3544,7 @@
         <v>6</v>
       </c>
       <c r="C88" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D88" t="s">
         <v>123</v>
@@ -3532,7 +3561,7 @@
         <v>7</v>
       </c>
       <c r="C89" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="90" spans="1:5">
@@ -3543,7 +3572,7 @@
         <v>89</v>
       </c>
       <c r="C90" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="D90" t="s">
         <v>123</v>
@@ -3560,7 +3589,7 @@
         <v>90</v>
       </c>
       <c r="C91" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="E91" t="s">
         <v>89</v>
@@ -3574,10 +3603,10 @@
         <v>91</v>
       </c>
       <c r="C92" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="E92" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="93" spans="1:5">
@@ -3588,10 +3617,10 @@
         <v>92</v>
       </c>
       <c r="C93" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="E93" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="94" spans="1:5">
@@ -3602,10 +3631,10 @@
         <v>93</v>
       </c>
       <c r="C94" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="E94" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="139.5">
@@ -3616,7 +3645,7 @@
         <v>94</v>
       </c>
       <c r="C95" s="12" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="96" spans="1:5">
@@ -3627,7 +3656,7 @@
         <v>95</v>
       </c>
       <c r="C96" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="97" spans="1:3">
@@ -3638,7 +3667,7 @@
         <v>96</v>
       </c>
       <c r="C97" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="98" spans="1:3">
@@ -3649,7 +3678,7 @@
         <v>97</v>
       </c>
       <c r="C98" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="99" spans="1:3">
@@ -3660,7 +3689,7 @@
         <v>98</v>
       </c>
       <c r="C99" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="100" spans="1:3">
@@ -3671,7 +3700,7 @@
         <v>99</v>
       </c>
       <c r="C100" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="101" spans="1:3">
@@ -3682,7 +3711,7 @@
         <v>100</v>
       </c>
       <c r="C101" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="102" spans="1:3">
@@ -3693,7 +3722,7 @@
         <v>101</v>
       </c>
       <c r="C102" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="103" spans="1:3">
@@ -3704,7 +3733,7 @@
         <v>102</v>
       </c>
       <c r="C103" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="104" spans="1:3">
@@ -3715,7 +3744,7 @@
         <v>103</v>
       </c>
       <c r="C104" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="105" spans="1:3">
@@ -3726,7 +3755,7 @@
         <v>104</v>
       </c>
       <c r="C105" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="106" spans="1:3">
@@ -3737,7 +3766,7 @@
         <v>105</v>
       </c>
       <c r="C106" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="107" spans="1:3">
@@ -3748,7 +3777,7 @@
         <v>106</v>
       </c>
       <c r="C107" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row r="108" spans="1:3">
@@ -3759,7 +3788,7 @@
         <v>107</v>
       </c>
       <c r="C108" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="109" spans="1:3">
@@ -3770,7 +3799,7 @@
         <v>108</v>
       </c>
       <c r="C109" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="110" spans="1:3">
@@ -3781,7 +3810,7 @@
         <v>109</v>
       </c>
       <c r="C110" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="111" spans="1:3">
@@ -3792,7 +3821,7 @@
         <v>110</v>
       </c>
       <c r="C111" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="46.5">
@@ -3803,7 +3832,7 @@
         <v>111</v>
       </c>
       <c r="C112" s="12" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="77.5">
@@ -3814,7 +3843,7 @@
         <v>112</v>
       </c>
       <c r="C113" s="11" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="114" spans="1:3">
@@ -3825,7 +3854,7 @@
         <v>113</v>
       </c>
       <c r="C114" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="115" spans="1:3">
@@ -3836,7 +3865,7 @@
         <v>114</v>
       </c>
       <c r="C115" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="116" spans="1:3">
@@ -3847,7 +3876,7 @@
         <v>115</v>
       </c>
       <c r="C116" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="117" spans="1:3">
@@ -3858,7 +3887,7 @@
         <v>116</v>
       </c>
       <c r="C117" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="118" spans="1:3">
@@ -3869,7 +3898,7 @@
         <v>117</v>
       </c>
       <c r="C118" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="119" spans="1:3">
@@ -3880,7 +3909,7 @@
         <v>118</v>
       </c>
       <c r="C119" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="120" spans="1:3">
@@ -3891,7 +3920,7 @@
         <v>119</v>
       </c>
       <c r="C120" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="123" spans="1:3">
@@ -4384,16 +4413,16 @@
         <v>322</v>
       </c>
       <c r="B3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D3" t="s">
         <v>120</v>
       </c>
       <c r="E3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F3" s="9"/>
     </row>
@@ -4402,21 +4431,21 @@
         <v>322</v>
       </c>
       <c r="B4" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C4" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D4" t="s">
         <v>120</v>
       </c>
       <c r="E4" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
   </sheetData>
@@ -4458,13 +4487,13 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D2" t="s">
         <v>120</v>
@@ -4475,27 +4504,27 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B3" t="s">
         <v>312</v>
       </c>
       <c r="C3" t="s">
+        <v>340</v>
+      </c>
+      <c r="E3" t="s">
         <v>341</v>
-      </c>
-      <c r="E3" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B4" t="s">
+        <v>342</v>
+      </c>
+      <c r="C4" t="s">
         <v>343</v>
-      </c>
-      <c r="C4" t="s">
-        <v>344</v>
       </c>
       <c r="E4">
         <v>1827</v>
@@ -4503,38 +4532,38 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B5" t="s">
         <v>110</v>
       </c>
       <c r="C5" t="s">
+        <v>345</v>
+      </c>
+      <c r="D5" t="s">
+        <v>347</v>
+      </c>
+      <c r="E5" t="s">
         <v>346</v>
-      </c>
-      <c r="D5" t="s">
-        <v>348</v>
-      </c>
-      <c r="E5" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B6" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B7" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C7" t="s">
         <v>317</v>
@@ -4548,50 +4577,50 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B8" t="s">
         <v>109</v>
       </c>
       <c r="C8" t="s">
+        <v>350</v>
+      </c>
+      <c r="D8" t="s">
         <v>351</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>352</v>
-      </c>
-      <c r="E8" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B9" t="s">
+        <v>358</v>
+      </c>
+      <c r="C9" t="s">
         <v>359</v>
-      </c>
-      <c r="C9" t="s">
-        <v>360</v>
       </c>
       <c r="D9" t="s">
         <v>139</v>
       </c>
       <c r="E9" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B10" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C10" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D10" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E10">
         <v>81323</v>
@@ -4599,16 +4628,16 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B11" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C11" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D11" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E11">
         <v>3221</v>
@@ -4621,10 +4650,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71749091-3478-4FCF-AAC9-EF5CE4F196A6}">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="A22" sqref="A22:E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5"/>
@@ -4655,18 +4684,18 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="B3" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C3" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E3">
         <v>9024</v>
@@ -4674,13 +4703,13 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="B4" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C4" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -4688,46 +4717,46 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="B5" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C5" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E5" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="5" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="B7" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C7" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E7" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="B8" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C8" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E8">
         <v>29133</v>
@@ -4735,13 +4764,13 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="B9" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C9" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E9">
         <v>3116</v>
@@ -4749,102 +4778,102 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="B10" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C10" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E10" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="B11" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C11" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E11" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="B12" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C12" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E12" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="B13" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C13" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E13" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="B14" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C14" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E14" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="5" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="B16" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C16" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E16" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="B17" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C17" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="E17">
         <v>29133</v>
@@ -4852,13 +4881,13 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="B18" t="s">
+        <v>401</v>
+      </c>
+      <c r="C18" t="s">
         <v>402</v>
-      </c>
-      <c r="C18" t="s">
-        <v>403</v>
       </c>
       <c r="E18">
         <v>3116</v>
@@ -4866,68 +4895,101 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="B19" t="s">
-        <v>404</v>
-      </c>
-      <c r="C19" t="s">
-        <v>406</v>
-      </c>
-      <c r="E19" t="s">
-        <v>388</v>
+        <v>466</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>467</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>453</v>
-      </c>
-      <c r="B20" t="s">
+        <v>451</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>469</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>451</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>470</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>451</v>
+      </c>
+      <c r="B22" t="s">
+        <v>403</v>
+      </c>
+      <c r="C22" t="s">
         <v>405</v>
       </c>
-      <c r="C20" t="s">
-        <v>407</v>
-      </c>
-      <c r="E20" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="5" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="5" t="s">
-        <v>410</v>
+      <c r="E22" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="B23" t="s">
+        <v>404</v>
+      </c>
+      <c r="C23" t="s">
+        <v>406</v>
+      </c>
+      <c r="E23" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="5" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="5" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
+        <v>451</v>
+      </c>
+      <c r="B26" t="s">
+        <v>409</v>
+      </c>
+      <c r="C26" t="s">
+        <v>412</v>
+      </c>
+      <c r="E26" t="s">
         <v>411</v>
       </c>
-      <c r="C23" t="s">
-        <v>414</v>
-      </c>
-      <c r="E23" t="s">
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" t="s">
+        <v>451</v>
+      </c>
+      <c r="B27" t="s">
+        <v>410</v>
+      </c>
+      <c r="C27" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" t="s">
-        <v>453</v>
-      </c>
-      <c r="B24" t="s">
-        <v>412</v>
-      </c>
-      <c r="C24" t="s">
-        <v>415</v>
-      </c>
-      <c r="E24" t="s">
-        <v>413</v>
+      <c r="E27" t="s">
+        <v>411</v>
       </c>
     </row>
   </sheetData>

</xml_diff>